<commit_message>
feat(budget): change template buget file
</commit_message>
<xml_diff>
--- a/Programming/WebFrontEnd/public/files/template-budget.xlsx
+++ b/Programming/WebFrontEnd/public/files/template-budget.xlsx
@@ -20,21 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Budget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Work ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currency</t>
+    <t xml:space="preserve">Sub Budget Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Budget Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency Name</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
@@ -344,17 +356,20 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="104" zoomScaleNormal="104" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="104" zoomScaleNormal="104" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,16 +397,32 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>